<commit_message>
register test using hashmap
</commit_message>
<xml_diff>
--- a/PROJECT_AUTOMATION/src/test/resources/testdata/project.xlsx
+++ b/PROJECT_AUTOMATION/src/test/resources/testdata/project.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login_allcase_data" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -75,6 +75,12 @@
     <t xml:space="preserve">March </t>
   </si>
   <si>
+    <t xml:space="preserve">santa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">santa+1@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">firstname</t>
   </si>
   <si>
@@ -84,7 +90,7 @@
     <t xml:space="preserve">emailid</t>
   </si>
   <si>
-    <t xml:space="preserve">country(take from the wepage because dropdown)</t>
+    <t xml:space="preserve">country</t>
   </si>
   <si>
     <t xml:space="preserve">city</t>
@@ -115,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -151,11 +157,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,8 +244,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -267,7 +276,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="2" sqref="H1 H2 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,10 +346,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="2" sqref="H1 H2 I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -408,9 +417,39 @@
         <v>123456</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>2003</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>123456</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="santa@gmail.com"/>
+    <hyperlink ref="G3" r:id="rId2" display="santa+1@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -427,46 +466,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="H1 H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="25.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,20 +519,30 @@
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="9" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2" s="4" t="n">
         <v>600000</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>123456789</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>